<commit_message>
Solve and calibrate not good
</commit_message>
<xml_diff>
--- a/tests/data/titration_table.xlsx
+++ b/tests/data/titration_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mphum\GitHub\calkulate\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E16234DA-63A4-40C1-9A08-25615226C535}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{224CEC5B-D850-4E7D-AFB3-B0704913975D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -43,6 +43,9 @@
     <t>analyte_mass</t>
   </si>
   <si>
+    <t>dic</t>
+  </si>
+  <si>
     <t>total_phosphate</t>
   </si>
   <si>
@@ -58,6 +61,9 @@
     <t>total_sulfate</t>
   </si>
   <si>
+    <t>opt_total_borate</t>
+  </si>
+  <si>
     <t>titrant_concentration</t>
   </si>
   <si>
@@ -70,19 +76,19 @@
     <t>alkalinity_certified</t>
   </si>
   <si>
+    <t>k_borate</t>
+  </si>
+  <si>
     <t>k_carbonic_1</t>
   </si>
   <si>
     <t>k_carbonic_2</t>
   </si>
   <si>
-    <t>k_phosphoric_1</t>
-  </si>
-  <si>
-    <t>k_phosphoric_2</t>
-  </si>
-  <si>
-    <t>k_phosphoric_3</t>
+    <t>k_fluoride</t>
+  </si>
+  <si>
+    <t>k_bisulfate</t>
   </si>
   <si>
     <t>k_water</t>
@@ -97,9 +103,21 @@
     <t>tests/data/</t>
   </si>
   <si>
+    <t>seawater-CRM-144.dat</t>
+  </si>
+  <si>
     <t>NaN</t>
   </si>
   <si>
+    <t>filename-does-not-exist.dat</t>
+  </si>
+  <si>
+    <t>seawater-CRM-144-function.dat</t>
+  </si>
+  <si>
+    <t>seawater-CRM-144-method.dat</t>
+  </si>
+  <si>
     <t>pH</t>
   </si>
   <si>
@@ -112,31 +130,13 @@
     <t>Dickson-1981-pH-with_phosphate.dat</t>
   </si>
   <si>
-    <t>seawater-CRM-144.dat</t>
-  </si>
-  <si>
-    <t>seawater-CRM-144-function.dat</t>
-  </si>
-  <si>
-    <t>seawater-CRM-144-method.dat</t>
-  </si>
-  <si>
-    <t>k_borate</t>
-  </si>
-  <si>
-    <t>k_fluoride</t>
-  </si>
-  <si>
-    <t>k_bisulfate</t>
-  </si>
-  <si>
-    <t>dic</t>
-  </si>
-  <si>
-    <t>opt_total_borate</t>
-  </si>
-  <si>
-    <t>filename-does-not-exist.dat</t>
+    <t>k_phosphate_1</t>
+  </si>
+  <si>
+    <t>k_phosphate_2</t>
+  </si>
+  <si>
+    <t>k_phosphate_3</t>
   </si>
 </sst>
 </file>
@@ -980,12 +980,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1010,67 +1009,67 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="Y1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" t="s">
-        <v>34</v>
-      </c>
-      <c r="W1" t="s">
-        <v>35</v>
-      </c>
-      <c r="X1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>19</v>
-      </c>
       <c r="Z1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="AA1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="AB1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -1078,13 +1077,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>33.570999999999998</v>
@@ -1093,7 +1092,7 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H2">
         <v>2031.53</v>
@@ -1111,40 +1110,40 @@
         <v>0.1</v>
       </c>
       <c r="P2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R2">
         <v>2238.6</v>
       </c>
       <c r="S2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="T2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="U2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="V2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="W2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="X2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Y2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Z2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="AA2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
@@ -1152,13 +1151,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E3">
         <v>33.570999999999998</v>
@@ -1167,7 +1166,7 @@
         <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H3">
         <v>2031.53</v>
@@ -1185,40 +1184,40 @@
         <v>0.1</v>
       </c>
       <c r="P3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R3">
         <v>2238.6</v>
       </c>
       <c r="S3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="T3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="U3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="V3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="W3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="X3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Y3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Z3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="AA3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
@@ -1226,13 +1225,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>33.570999999999998</v>
@@ -1241,7 +1240,7 @@
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H4">
         <v>2031.53</v>
@@ -1259,40 +1258,40 @@
         <v>0.1</v>
       </c>
       <c r="P4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R4">
         <v>2238.6</v>
       </c>
       <c r="S4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="T4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="U4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="V4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="W4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="X4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Y4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Z4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="AA4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
@@ -1300,13 +1299,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5">
         <v>33.570999999999998</v>
@@ -1315,7 +1314,7 @@
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H5">
         <v>2031.53</v>
@@ -1336,13 +1335,13 @@
         <v>27082.6</v>
       </c>
       <c r="N5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O5">
         <v>0.1</v>
       </c>
       <c r="P5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q5">
         <v>25</v>
@@ -1351,31 +1350,31 @@
         <v>2238.6</v>
       </c>
       <c r="S5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="T5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="U5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="V5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="W5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="X5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Y5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Z5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="AA5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
@@ -1383,19 +1382,19 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E6">
         <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>200</v>
@@ -1419,16 +1418,16 @@
         <v>28240</v>
       </c>
       <c r="N6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P6">
         <v>0.3</v>
       </c>
       <c r="Q6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R6">
         <v>2450</v>
@@ -1443,25 +1442,25 @@
         <v>8.1999999999999996E-10</v>
       </c>
       <c r="V6">
-        <v>2.4509803921568601E-3</v>
+        <v>2.4509800000000002E-3</v>
       </c>
       <c r="W6">
-        <v>8.1300813008129996E-2</v>
+        <v>8.1300813E-2</v>
       </c>
       <c r="X6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Y6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Z6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="AA6" s="1">
         <v>4.3200000000000001E-14</v>
       </c>
       <c r="AB6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
@@ -1469,19 +1468,19 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G7">
         <v>200</v>
@@ -1505,16 +1504,16 @@
         <v>28240</v>
       </c>
       <c r="N7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="O7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="P7">
         <v>0.3</v>
       </c>
       <c r="Q7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="R7">
         <v>2450</v>
@@ -1529,13 +1528,13 @@
         <v>8.1999999999999996E-10</v>
       </c>
       <c r="V7">
-        <v>2.4509803921568601E-3</v>
+        <v>2.4509800000000002E-3</v>
       </c>
       <c r="W7">
-        <v>8.1300813008129996E-2</v>
+        <v>8.1300813E-2</v>
       </c>
       <c r="X7">
-        <v>1.7605633802816899E-2</v>
+        <v>1.7605633999999998E-2</v>
       </c>
       <c r="Y7" s="1">
         <v>7.9999999999999996E-7</v>
@@ -1547,7 +1546,7 @@
         <v>4.3200000000000001E-14</v>
       </c>
       <c r="AB7" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add batch mean molinity function
</commit_message>
<xml_diff>
--- a/tests/data/titration_table.xlsx
+++ b/tests/data/titration_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mphum\GitHub\calkulate\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{224CEC5B-D850-4E7D-AFB3-B0704913975D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EFCB966-7E08-4DD2-8A48-19B531078D9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -91,6 +91,15 @@
     <t>k_bisulfate</t>
   </si>
   <si>
+    <t>k_phosphate_1</t>
+  </si>
+  <si>
+    <t>k_phosphate_2</t>
+  </si>
+  <si>
+    <t>k_phosphate_3</t>
+  </si>
+  <si>
     <t>k_water</t>
   </si>
   <si>
@@ -128,15 +137,6 @@
   </si>
   <si>
     <t>Dickson-1981-pH-with_phosphate.dat</t>
-  </si>
-  <si>
-    <t>k_phosphate_1</t>
-  </si>
-  <si>
-    <t>k_phosphate_2</t>
-  </si>
-  <si>
-    <t>k_phosphate_3</t>
   </si>
 </sst>
 </file>
@@ -981,7 +981,7 @@
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,19 +1057,19 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -1077,13 +1077,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>33.570999999999998</v>
@@ -1092,7 +1092,7 @@
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H2">
         <v>2031.53</v>
@@ -1110,40 +1110,40 @@
         <v>0.1</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Q2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="R2">
         <v>2238.6</v>
       </c>
       <c r="S2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="T2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="V2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="W2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="X2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Y2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Z2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AA2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
@@ -1151,13 +1151,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E3">
         <v>33.570999999999998</v>
@@ -1166,7 +1166,7 @@
         <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H3">
         <v>2031.53</v>
@@ -1184,40 +1184,40 @@
         <v>0.1</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Q3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="R3">
         <v>2238.6</v>
       </c>
       <c r="S3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="T3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="V3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="W3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="X3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Y3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Z3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AA3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
@@ -1225,13 +1225,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <v>33.570999999999998</v>
@@ -1240,7 +1240,7 @@
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H4">
         <v>2031.53</v>
@@ -1258,40 +1258,40 @@
         <v>0.1</v>
       </c>
       <c r="P4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Q4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="R4">
         <v>2238.6</v>
       </c>
       <c r="S4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="T4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="V4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="W4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="X4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Y4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Z4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AA4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
@@ -1299,13 +1299,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E5">
         <v>33.570999999999998</v>
@@ -1314,7 +1314,7 @@
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H5">
         <v>2031.53</v>
@@ -1335,13 +1335,13 @@
         <v>27082.6</v>
       </c>
       <c r="N5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O5">
         <v>0.1</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Q5">
         <v>25</v>
@@ -1350,31 +1350,31 @@
         <v>2238.6</v>
       </c>
       <c r="S5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="T5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="V5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="W5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="X5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Y5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Z5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AA5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
@@ -1382,22 +1382,22 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G6">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="H6">
         <v>2200</v>
@@ -1418,16 +1418,16 @@
         <v>28240</v>
       </c>
       <c r="N6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P6">
         <v>0.3</v>
       </c>
       <c r="Q6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="R6">
         <v>2450</v>
@@ -1448,19 +1448,19 @@
         <v>8.1300813E-2</v>
       </c>
       <c r="X6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Y6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Z6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AA6" s="1">
         <v>4.3200000000000001E-14</v>
       </c>
       <c r="AB6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
@@ -1468,22 +1468,22 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E7">
         <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G7">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="H7">
         <v>2200</v>
@@ -1504,16 +1504,16 @@
         <v>28240</v>
       </c>
       <c r="N7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P7">
         <v>0.3</v>
       </c>
       <c r="Q7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="R7">
         <v>2450</v>
@@ -1546,7 +1546,7 @@
         <v>4.3200000000000001E-14</v>
       </c>
       <c r="AB7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>